<commit_message>
update table1 and fig legends
</commit_message>
<xml_diff>
--- a/table_1_2025_12_14.xlsx
+++ b/table_1_2025_12_14.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="353">
   <si>
     <t xml:space="preserve">83-type signature</t>
   </si>
@@ -1075,6 +1076,33 @@
   </si>
   <si>
     <t xml:space="preserve">CNS-hdp.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artefact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pole+MMRd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28m</t>
   </si>
 </sst>
 </file>
@@ -1287,115 +1315,115 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1408,6 +1436,23 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1651,7 +1696,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="9:9"/>
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="44:44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="13.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1664,7 +1709,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="18.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="18.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="21.55"/>
   </cols>
   <sheetData>
@@ -1705,1460 +1750,1457 @@
       <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="8" t="n">
+      <c r="K2" s="9" t="n">
         <v>0.982</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="8" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="8" t="n">
+      <c r="K3" s="9" t="n">
         <v>0.961</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="8" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="8" t="n">
+      <c r="K4" s="9" t="n">
         <v>0.936</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="D6" s="10"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="8" t="n">
+      <c r="K7" s="9" t="n">
         <v>0.906</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8" t="s">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="M8" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="0" t="s">
+      <c r="M9" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="8" t="n">
+      <c r="K10" s="9" t="n">
         <v>0.914</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="10" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="7" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K11" s="8" t="n">
+      <c r="K11" s="9" t="n">
         <v>0.954</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="8" t="n">
+      <c r="K12" s="9" t="n">
         <v>0.967</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8" t="s">
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="8" t="n">
+      <c r="K14" s="9" t="n">
         <v>0.936</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8" t="s">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="8" t="n">
+      <c r="K16" s="9" t="n">
         <v>0.974</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="K17" s="8" t="n">
+      <c r="K17" s="9" t="n">
         <v>0.952</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="0" t="s">
+      <c r="M17" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7" t="s">
+      <c r="D18" s="7"/>
+      <c r="E18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="K18" s="8" t="n">
+      <c r="K18" s="9" t="n">
         <v>0.944</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="L18" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="K19" s="8" t="n">
+      <c r="K19" s="9" t="n">
         <v>0.92</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="L19" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8" t="s">
+      <c r="J21" s="7"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="K23" s="8" t="n">
+      <c r="K23" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="L23" s="8" t="s">
+      <c r="L23" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="7" t="s">
+      <c r="D24" s="11"/>
+      <c r="E24" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="K24" s="8" t="n">
+      <c r="K24" s="9" t="n">
         <v>0.98</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="L24" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="K26" s="8" t="n">
+      <c r="K26" s="9" t="n">
         <v>0.99</v>
       </c>
-      <c r="L26" s="8" t="s">
+      <c r="L26" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8" t="s">
+      <c r="J27" s="7"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8" t="s">
+      <c r="F28" s="14"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8" t="s">
+      <c r="F29" s="14"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7" t="s">
+      <c r="D30" s="7"/>
+      <c r="E30" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H30" s="6" t="s">
+      <c r="H30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="6"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8" t="s">
+      <c r="K31" s="9"/>
+      <c r="L31" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="8" t="s">
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="K32" s="8" t="n">
+      <c r="K32" s="9" t="n">
         <v>0.965</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="L32" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G33" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H33" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J33" s="6"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8" t="s">
+      <c r="J33" s="7"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G34" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J34" s="6"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="H35" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J35" s="6"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8" t="s">
+      <c r="J35" s="7"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F36" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="I36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J36" s="6"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8" t="s">
+      <c r="J36" s="7"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G37" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="H37" s="6" t="s">
+      <c r="H37" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="I37" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J37" s="6"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8" t="s">
+      <c r="J37" s="7"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G38" s="13" t="s">
+      <c r="G38" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H38" s="6" t="s">
+      <c r="H38" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I38" s="6" t="s">
+      <c r="I38" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J38" s="6"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8" t="s">
+      <c r="J38" s="7"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="G39" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H39" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="I39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J39" s="6"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8" t="s">
+      <c r="J39" s="7"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="F40" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G40" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="H40" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I40" s="6" t="s">
+      <c r="I40" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="6"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F41" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G41" s="13" t="s">
+      <c r="G41" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="H41" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I41" s="6" t="s">
+      <c r="I41" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J41" s="6"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8" t="s">
+      <c r="J41" s="7"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M41" s="0" t="s">
+      <c r="M41" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="G42" s="13" t="s">
+      <c r="G42" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="H42" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I42" s="6" t="s">
+      <c r="I42" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J42" s="6"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="0" t="s">
+      <c r="J42" s="7"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="6" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6" t="s">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E43" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="F43" s="6"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8" t="s">
+      <c r="F43" s="7"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M43" s="0" t="s">
+      <c r="M43" s="6" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="F44" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G44" s="13" t="s">
+      <c r="G44" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H44" s="6" t="s">
+      <c r="H44" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I44" s="6" t="s">
+      <c r="I44" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J44" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="K44" s="8" t="n">
+      <c r="K44" s="9" t="n">
         <v>0.97</v>
       </c>
-      <c r="L44" s="8"/>
+      <c r="L44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G45" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H45" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="I45" s="6" t="s">
+      <c r="I45" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="J45" s="6"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E46" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F46" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G46" s="13" t="s">
+      <c r="G46" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H46" s="6" t="s">
+      <c r="H46" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I46" s="6" t="s">
+      <c r="I46" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J46" s="6"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8" t="s">
+      <c r="J46" s="7"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M46" s="0" t="s">
+      <c r="M46" s="6" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="F47" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="G47" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H47" s="13" t="s">
+      <c r="H47" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I47" s="6" t="s">
+      <c r="I47" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J47" s="8" t="s">
+      <c r="J47" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="K47" s="8" t="n">
+      <c r="K47" s="9" t="n">
         <v>0.93</v>
       </c>
-      <c r="L47" s="8" t="s">
+      <c r="L47" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M47" s="0" t="s">
+      <c r="M47" s="6" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J48" s="9" t="n">
-        <f aca="false">COUNTBLANK(J2:J47)</f>
-        <v>28</v>
-      </c>
+      <c r="J48" s="10"/>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
-      <c r="K50" s="15"/>
-      <c r="L50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="17"/>
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="17"/>
-      <c r="K51" s="17"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17"/>
-      <c r="J52" s="17"/>
-      <c r="K52" s="17"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
     </row>
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="42">
@@ -3223,277 +3265,277 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="9:9 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="44:44 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="13.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="25.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="28.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="6" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="6" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="6" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="6" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="6" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="6" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="6" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="6" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="6" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="6" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="6" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="6" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="6" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="6" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="6" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="6" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="6" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="6" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="6" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="6" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="6" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="6" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="6" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="6" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="6" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="6" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="6" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="6" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="6" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="6" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="6" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="6" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="6" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="6" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="6" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="6" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="6" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="6" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="6" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="6" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="6" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="6" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="6" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="6" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="6" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="6" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="6" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="6" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -3516,507 +3558,507 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="9:9 E13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="44:44 E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="11.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="17.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="19" width="9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="19" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="17.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="20" width="8.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="C10" s="22" t="n">
+      <c r="C10" s="23" t="n">
         <v>0.8971999</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="C11" s="22" t="n">
+      <c r="C11" s="23" t="n">
         <v>0.9275639</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="C12" s="22" t="n">
+      <c r="C12" s="23" t="n">
         <v>0.9334432</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="C13" s="22" t="n">
+      <c r="C13" s="23" t="n">
         <v>0.9338192</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="C14" s="22" t="n">
+      <c r="C14" s="23" t="n">
         <v>0.9348804</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="C15" s="22" t="n">
+      <c r="C15" s="23" t="n">
         <v>0.942874</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="C16" s="22" t="n">
+      <c r="C16" s="23" t="n">
         <v>0.9504778</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="C17" s="22" t="n">
+      <c r="C17" s="23" t="n">
         <v>0.9508531</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="C18" s="22" t="n">
+      <c r="C18" s="23" t="n">
         <v>0.9509863</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="C19" s="22" t="n">
+      <c r="C19" s="23" t="n">
         <v>0.9596999</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="C20" s="22" t="n">
+      <c r="C20" s="23" t="n">
         <v>0.9653861</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="C21" s="22" t="n">
+      <c r="C21" s="23" t="n">
         <v>0.9657092</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="C22" s="22" t="n">
+      <c r="C22" s="23" t="n">
         <v>0.9659186</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="C23" s="22" t="n">
+      <c r="C23" s="23" t="n">
         <v>0.9687676</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="C24" s="22" t="n">
+      <c r="C24" s="23" t="n">
         <v>0.9705652</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="C25" s="22" t="n">
+      <c r="C25" s="23" t="n">
         <v>0.9727932</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="C26" s="22" t="n">
+      <c r="C26" s="23" t="n">
         <v>0.9742897</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="C27" s="22" t="n">
+      <c r="C27" s="23" t="n">
         <v>0.98</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="C28" s="22" t="n">
+      <c r="C28" s="23" t="n">
         <v>0.9802872</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="C29" s="22" t="n">
+      <c r="C29" s="23" t="n">
         <v>0.9819073</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="22" t="s">
         <v>294</v>
       </c>
-      <c r="C30" s="22" t="n">
+      <c r="C30" s="23" t="n">
         <v>0.9828072</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="C31" s="22" t="n">
+      <c r="C31" s="23" t="n">
         <v>0.9828327</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="C32" s="22" t="n">
+      <c r="C32" s="23" t="n">
         <v>0.9833134</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="C33" s="22" t="n">
+      <c r="C33" s="23" t="n">
         <v>0.9866623</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="22" t="s">
         <v>298</v>
       </c>
-      <c r="C34" s="22" t="n">
+      <c r="C34" s="23" t="n">
         <v>0.9894299</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="C35" s="22" t="n">
+      <c r="C35" s="23" t="n">
         <v>0.9915474</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="C36" s="22" t="n">
+      <c r="C36" s="23" t="n">
         <v>0.9928565</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="C37" s="22" t="n">
+      <c r="C37" s="23" t="n">
         <v>0.9932411</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="C38" s="22" t="n">
+      <c r="C38" s="23" t="n">
         <v>0.9948542</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="C39" s="22" t="n">
+      <c r="C39" s="23" t="n">
         <v>0.9951084</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="21" t="s">
+      <c r="A40" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="C40" s="22" t="n">
+      <c r="C40" s="23" t="n">
         <v>0.9971654</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="C41" s="22" t="n">
+      <c r="C41" s="23" t="n">
         <v>0.9978364</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="C42" s="22" t="n">
+      <c r="C42" s="23" t="n">
         <v>0.9978427</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="C43" s="22" t="n">
+      <c r="C43" s="23" t="n">
         <v>0.9978611</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="C44" s="22" t="n">
+      <c r="C44" s="23" t="n">
         <v>0.9980734</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="C45" s="22" t="n">
+      <c r="C45" s="23" t="n">
         <v>0.9990591</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="C46" s="22" t="n">
+      <c r="C46" s="23" t="n">
         <v>0.9999559</v>
       </c>
     </row>
@@ -4039,17 +4081,17 @@
   <dimension ref="B1:E46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="9:9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="44:44 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="13.5" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="23" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="9.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="8.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="24" t="s">
@@ -4057,7 +4099,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="25" t="s">
@@ -4065,7 +4107,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="24" t="s">
@@ -4073,17 +4115,17 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="24" t="s">
@@ -4092,7 +4134,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="24"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -4100,7 +4142,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="24" t="s">
@@ -4108,12 +4150,12 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D10" s="24" t="s">
@@ -4121,7 +4163,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="24" t="s">
@@ -4130,13 +4172,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="26"/>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="24"/>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="27" t="s">
@@ -4144,7 +4186,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>63</v>
       </c>
       <c r="D14" s="27" t="s">
@@ -4152,7 +4194,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D15" s="24" t="s">
@@ -4160,7 +4202,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D16" s="24" t="s">
@@ -4168,7 +4210,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D17" s="24" t="s">
@@ -4176,7 +4218,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="24" t="s">
@@ -4184,12 +4226,12 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D20" s="24" t="s">
@@ -4197,7 +4239,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="24" t="s">
@@ -4205,7 +4247,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D22" s="25" t="s">
@@ -4213,7 +4255,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="11" t="s">
         <v>97</v>
       </c>
       <c r="D23" s="24" t="s">
@@ -4221,7 +4263,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D24" s="24" t="s">
@@ -4229,7 +4271,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>105</v>
       </c>
       <c r="D25" s="24" t="s">
@@ -4237,12 +4279,12 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>111</v>
       </c>
       <c r="D27" s="24" t="s">
@@ -4250,12 +4292,12 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="7" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>116</v>
       </c>
       <c r="D29" s="24" t="s">
@@ -4263,22 +4305,22 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="7" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="7" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="11" t="s">
         <v>136</v>
       </c>
       <c r="D33" s="28" t="s">
@@ -4286,7 +4328,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>141</v>
       </c>
       <c r="D34" s="24" t="s">
@@ -4294,7 +4336,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="7" t="s">
         <v>146</v>
       </c>
       <c r="D35" s="24" t="s">
@@ -4302,7 +4344,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="7" t="s">
         <v>151</v>
       </c>
       <c r="D36" s="24" t="s">
@@ -4310,7 +4352,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="7" t="s">
         <v>156</v>
       </c>
       <c r="D37" s="24" t="s">
@@ -4318,12 +4360,12 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="11" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="7" t="s">
         <v>166</v>
       </c>
       <c r="D39" s="24" t="s">
@@ -4331,7 +4373,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D40" s="27" t="s">
@@ -4339,39 +4381,39 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D41" s="6" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="6" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" s="6" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="6" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D45" s="27" t="s">
@@ -4379,7 +4421,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="7" t="s">
         <v>203</v>
       </c>
       <c r="D46" s="24" t="s">
@@ -4395,4 +4437,364 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C79"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B41" activeCellId="1" sqref="44:44 B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7"/>
+      <c r="B8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9"/>
+      <c r="B14" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9"/>
+      <c r="B15" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9"/>
+      <c r="B19" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9"/>
+      <c r="B21" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9"/>
+      <c r="B22" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9"/>
+      <c r="B23" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9"/>
+      <c r="B26" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9"/>
+      <c r="B27" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9"/>
+      <c r="B28" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9"/>
+      <c r="B29" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9"/>
+      <c r="B30" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9"/>
+      <c r="B31" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9"/>
+      <c r="B33" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9"/>
+      <c r="B34" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9"/>
+      <c r="B35" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="9"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="7"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="7"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="7"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="7"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="7"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="7"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="7"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="7"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="7"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="7"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="7"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="7"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="7"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="7"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="7"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="7"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="7"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="7"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="7"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>